<commit_message>
Elektrikli atık toplama aracı rotalama sistemi için temel uygulama dosyaları eklendi. Yeni dosyalar arasında ARP ve VRP algoritmalarını içeren Python dosyaları ile atık toplama noktaları ve şarj istasyonları için harita görselleştirmesi yapan HTML dosyası bulunmaktadır. Ayrıca, Excel dosyası güncellenmiştir.
</commit_message>
<xml_diff>
--- a/talep_noktalari_guncellenmis.xlsx
+++ b/talep_noktalari_guncellenmis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sefed\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE773E6D-AD88-4BA0-BD52-EE2334485E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07C6500-AADE-485E-989B-2A9060E3BF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -521,14 +521,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -550,10 +551,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>28.606909999999999</v>
+        <v>30.571129614119499</v>
       </c>
       <c r="C2">
-        <v>41.829948000000002</v>
+        <v>37.769279149053801</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -561,10 +562,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>28.299790000000002</v>
+        <v>30.5361826961962</v>
       </c>
       <c r="C3">
-        <v>41.833523</v>
+        <v>37.771775382312597</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,10 +573,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>28.32122</v>
+        <v>30.5389666077598</v>
       </c>
       <c r="C4">
-        <v>41.821710000000003</v>
+        <v>37.761188746681299</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -583,10 +584,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>28.18618</v>
+        <v>30.5236449889832</v>
       </c>
       <c r="C5">
-        <v>41.821860999999998</v>
+        <v>37.761002874389298</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -594,10 +595,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>28.24643</v>
+        <v>30.529855974324001</v>
       </c>
       <c r="C6">
-        <v>41.842658999999998</v>
+        <v>37.779874683269597</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -605,10 +606,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>28.488060000000001</v>
+        <v>30.5575996303048</v>
       </c>
       <c r="C7">
-        <v>41.831522</v>
+        <v>37.770417803341601</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -616,10 +617,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>28.720089999999999</v>
+        <v>30.5844729616467</v>
       </c>
       <c r="C8">
-        <v>41.812728999999997</v>
+        <v>37.754037659258501</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -627,10 +628,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>28.374300000000002</v>
+        <v>30.5447728310508</v>
       </c>
       <c r="C9">
-        <v>41.828913</v>
+        <v>37.767800183154101</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -638,10 +639,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>28.399339999999999</v>
+        <v>30.547244452117098</v>
       </c>
       <c r="C10">
-        <v>41.841304000000001</v>
+        <v>37.779017089329699</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -649,10 +650,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>28.587409999999998</v>
+        <v>30.5691474941673</v>
       </c>
       <c r="C11">
-        <v>41.822152000000003</v>
+        <v>37.7622131223577</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -660,10 +661,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>28.106010000000001</v>
+        <v>30.5141888528279</v>
       </c>
       <c r="C12">
-        <v>41.833908999999998</v>
+        <v>37.7716603420279</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -671,10 +672,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>28.657440000000001</v>
+        <v>30.577454360126399</v>
       </c>
       <c r="C13">
-        <v>41.809762999999997</v>
+        <v>37.751220040101103</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -682,10 +683,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>28.583110000000001</v>
+        <v>30.568844942782199</v>
       </c>
       <c r="C14">
-        <v>41.815843000000001</v>
+        <v>37.756521403605703</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -693,10 +694,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>28.430350000000001</v>
+        <v>30.551185439043099</v>
       </c>
       <c r="C15">
-        <v>41.827088000000003</v>
+        <v>37.766288686695098</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -704,10 +705,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>28.47513</v>
+        <v>30.556713370143498</v>
       </c>
       <c r="C16">
-        <v>41.811948999999998</v>
+        <v>37.752762017912502</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -715,10 +716,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>28.253270000000001</v>
+        <v>30.530804076422001</v>
       </c>
       <c r="C17">
-        <v>41.836896000000003</v>
+        <v>37.774701114365399</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -726,10 +727,10 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>28.32863</v>
+        <v>30.539632039744699</v>
       </c>
       <c r="C18">
-        <v>41.827570700000003</v>
+        <v>37.766483263108498</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -737,10 +738,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>28.537120999999999</v>
+        <v>30.5637164423968</v>
       </c>
       <c r="C19">
-        <v>41.812888999999998</v>
+        <v>37.753754189679299</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -748,10 +749,10 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>28.505569999999999</v>
+        <v>30.559690847465401</v>
       </c>
       <c r="C20">
-        <v>41.827992000000002</v>
+        <v>37.767280652146503</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -759,10 +760,10 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>28.100439999999999</v>
+        <v>30.5118347246543</v>
       </c>
       <c r="C21">
-        <v>41.890914000000002</v>
+        <v>37.822978285942398</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -770,10 +771,10 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>28.079370000000001</v>
+        <v>30.5113974779971</v>
       </c>
       <c r="C22">
-        <v>41.826261000000002</v>
+        <v>37.7647096216254</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -781,10 +782,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>28.577459999999999</v>
+        <v>30.5683081539031</v>
       </c>
       <c r="C23">
-        <v>41.812336999999999</v>
+        <v>37.753351753282701</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -792,10 +793,10 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>28.414895213426099</v>
+        <v>30.549538582467701</v>
       </c>
       <c r="C24">
-        <v>41.823500723167299</v>
+        <v>37.763022249616903</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -803,10 +804,10 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>28.3555497534688</v>
+        <v>30.540978586743101</v>
       </c>
       <c r="C25">
-        <v>41.884755843902703</v>
+        <v>37.818041546542801</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -814,10 +815,10 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>28.455760614336601</v>
+        <v>30.5534791459276</v>
       </c>
       <c r="C26">
-        <v>41.846905874972201</v>
+        <v>37.784194969271702</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -825,10 +826,10 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>28.4670211934083</v>
+        <v>30.555468197129201</v>
       </c>
       <c r="C27">
-        <v>41.822929642686297</v>
+        <v>37.762630857656397</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -836,10 +837,10 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>28.246677700108599</v>
+        <v>30.530786306680898</v>
       </c>
       <c r="C28">
-        <v>41.812533226021998</v>
+        <v>37.752747616298102</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -847,10 +848,10 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>28.386871411990199</v>
+        <v>30.546587789673001</v>
       </c>
       <c r="C29">
-        <v>41.815841738125002</v>
+        <v>37.756059268715099</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -858,10 +859,10 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>28.299990629722799</v>
+        <v>30.535705602700201</v>
       </c>
       <c r="C30">
-        <v>41.8502345951607</v>
+        <v>37.7868239178745</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -869,10 +870,10 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>28.629373345457498</v>
+        <v>30.574031880106201</v>
       </c>
       <c r="C31">
-        <v>41.817904447700499</v>
+        <v>37.758486366691898</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -880,10 +881,10 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>28.5066080958517</v>
+        <v>30.560003340186</v>
       </c>
       <c r="C32">
-        <v>41.821416824962299</v>
+        <v>37.761361556970101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -891,10 +892,10 @@
         <v>34</v>
       </c>
       <c r="B33">
-        <v>28.4651971159795</v>
+        <v>30.5553639935451</v>
       </c>
       <c r="C33">
-        <v>41.819466438069199</v>
+        <v>37.7595079328201</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -902,10 +903,10 @@
         <v>35</v>
       </c>
       <c r="B34">
-        <v>28.461178028400301</v>
+        <v>30.554745651158399</v>
       </c>
       <c r="C34">
-        <v>41.824944030111503</v>
+        <v>37.7644310623444</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -913,10 +914,10 @@
         <v>36</v>
       </c>
       <c r="B35">
-        <v>28.417239105665299</v>
+        <v>30.548960566148899</v>
       </c>
       <c r="C35">
-        <v>41.8518734829252</v>
+        <v>37.788577392911101</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -924,10 +925,10 @@
         <v>37</v>
       </c>
       <c r="B36">
-        <v>28.5191747506321</v>
+        <v>30.560898048450799</v>
       </c>
       <c r="C36">
-        <v>41.839350164133798</v>
+        <v>37.777540282213003</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -935,10 +936,10 @@
         <v>38</v>
       </c>
       <c r="B37">
-        <v>28.542970770818201</v>
+        <v>30.5640707909029</v>
       </c>
       <c r="C37">
-        <v>41.823349731882502</v>
+        <v>37.7631876423035</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -946,10 +947,10 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <v>28.696602780648099</v>
+        <v>30.579623569627199</v>
       </c>
       <c r="C38">
-        <v>41.887134232054699</v>
+        <v>37.820985760366199</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -957,10 +958,10 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>28.4729450162768</v>
+        <v>30.5563440888914</v>
       </c>
       <c r="C39">
-        <v>41.816049200458103</v>
+        <v>37.756448928897001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -968,10 +969,10 @@
         <v>41</v>
       </c>
       <c r="B40">
-        <v>28.440836087461999</v>
+        <v>30.552646713805501</v>
       </c>
       <c r="C40">
-        <v>41.817921078642101</v>
+        <v>37.7580589495252</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -979,10 +980,10 @@
         <v>42</v>
       </c>
       <c r="B41">
-        <v>28.763070602597601</v>
+        <v>30.5892163509704</v>
       </c>
       <c r="C41">
-        <v>41.817230933802897</v>
+        <v>37.758191214288701</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -990,10 +991,10 @@
         <v>43</v>
       </c>
       <c r="B42">
-        <v>28.567303807097101</v>
+        <v>30.566017308161701</v>
       </c>
       <c r="C42">
-        <v>41.850899599646603</v>
+        <v>37.788053650556101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>